<commit_message>
updated large codeword set with all words capital
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data/91codewords.xlsx
+++ b/Documentation/Sample Data/91codewords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Desktop\Project\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D360B2-764B-4371-91B9-285A1A3F38B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D0C5A3-622D-4526-B0E4-E2D16A81208C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9C9CA1DB-B53F-4F86-B663-5B30F3274407}"/>
   </bookViews>
@@ -670,7 +670,7 @@
   <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A353" sqref="A353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
implemented codword smilarity logic
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data/91codewords.xlsx
+++ b/Documentation/Sample Data/91codewords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Desktop\Codeword\Codeword-GDPII\Documentation\Sample Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP II\Codeword-GDPII\Documentation\Sample Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778B4D77-D9E7-41D0-97A2-F1BBB115F553}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC3C890-398B-49F9-9AD4-0899C92BF1BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{9C9CA1DB-B53F-4F86-B663-5B30F3274407}"/>
   </bookViews>
@@ -344,12 +344,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BD555D-849D-4A7D-847C-A1A487A0923A}">
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:XFD96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,15 +1226,6 @@
       </c>
       <c r="B92" s="1"/>
     </row>
-    <row r="93" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A93" s="2"/>
-    </row>
-    <row r="94" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="95" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>